<commit_message>
Updated Gameboard og backlog
</commit_message>
<xml_diff>
--- a/ProductBacklog_v.29.10.xlsx
+++ b/ProductBacklog_v.29.10.xlsx
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>Score</t>
   </si>
@@ -310,6 +310,42 @@
   </si>
   <si>
     <t>Revideret 29/10 kl. 13:50</t>
+  </si>
+  <si>
+    <t>Ansvarsperson(er)</t>
+  </si>
+  <si>
+    <t>Peter R., Dan R</t>
+  </si>
+  <si>
+    <t>Jannik E., Marcus M., Elinor M., Emil N., Niki T.</t>
+  </si>
+  <si>
+    <t>Markus S., Peter B.</t>
+  </si>
+  <si>
+    <t>Marcus M., Emil N.</t>
+  </si>
+  <si>
+    <t>Peter R., Jannik E., Dan R.</t>
+  </si>
+  <si>
+    <t>Peter R., Jannik E., Marcus M.</t>
+  </si>
+  <si>
+    <t>Peter R., Niki T., Jannik E.</t>
+  </si>
+  <si>
+    <t>Peter R., Jannik E., Marcus M., Dan R.</t>
+  </si>
+  <si>
+    <t>Elinor M.</t>
+  </si>
+  <si>
+    <t>Emil N., Marcus M.</t>
+  </si>
+  <si>
+    <t>Emil N.</t>
   </si>
 </sst>
 </file>
@@ -740,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,11 +788,13 @@
     <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="4.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="39.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="22.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
@@ -764,10 +802,13 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>43</v>
       </c>
@@ -778,56 +819,56 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="2"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
@@ -838,7 +879,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
@@ -847,9 +888,11 @@
       <c r="D11" s="6">
         <v>39</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
@@ -858,9 +901,11 @@
       <c r="D12" s="6">
         <v>73</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>7</v>
       </c>
@@ -869,16 +914,18 @@
       <c r="D13" s="6">
         <v>12</v>
       </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>12</v>
       </c>
@@ -887,7 +934,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -896,7 +943,9 @@
       <c r="D16" s="6">
         <v>30</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
@@ -926,7 +975,9 @@
       <c r="D19" s="6">
         <v>5</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
@@ -937,7 +988,9 @@
       <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
@@ -948,7 +1001,9 @@
       <c r="D21" s="6">
         <v>1</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
@@ -975,7 +1030,9 @@
       <c r="D24" s="6">
         <v>0.5</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -986,7 +1043,9 @@
       <c r="D25" s="6">
         <v>0.5</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -997,7 +1056,9 @@
       <c r="D26" s="6">
         <v>2</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
@@ -1033,7 +1094,9 @@
       <c r="D30" s="6">
         <v>2</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -1044,7 +1107,9 @@
       <c r="D31" s="6">
         <v>2</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
@@ -1055,7 +1120,9 @@
       <c r="D32" s="6">
         <v>8</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
@@ -1066,7 +1133,9 @@
       <c r="D33" s="6">
         <v>2</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
@@ -1077,7 +1146,9 @@
       <c r="D34" s="6">
         <v>2</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
@@ -1088,7 +1159,9 @@
       <c r="D35" s="6">
         <v>3</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
@@ -1099,7 +1172,9 @@
       <c r="D36" s="6">
         <v>8</v>
       </c>
-      <c r="E36" s="6"/>
+      <c r="E36" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
@@ -1110,7 +1185,9 @@
       <c r="D37" s="6">
         <v>6</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
@@ -1163,7 +1240,9 @@
       <c r="D43" s="6">
         <v>5</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
@@ -1200,7 +1279,9 @@
       <c r="D47" s="6">
         <v>4</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
@@ -1233,7 +1314,9 @@
       <c r="D50" s="6">
         <v>2</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
@@ -1244,13 +1327,15 @@
       <c r="D51" s="6">
         <v>2</v>
       </c>
-      <c r="E51" s="6"/>
+      <c r="E51" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="4"/>
+      <c r="B52" s="2"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6">
         <v>1</v>

</xml_diff>